<commit_message>
All tests passing on Kayla's intel MacBook and on the ENKI server.
</commit_message>
<xml_diff>
--- a/tests/testsave.xlsx
+++ b/tests/testsave.xlsx
@@ -608,7 +608,7 @@
         <v>62.5</v>
       </c>
       <c r="U2" t="n">
-        <v>1299</v>
+        <v>1299.09471</v>
       </c>
     </row>
     <row r="3">
@@ -679,7 +679,7 @@
         <v>128</v>
       </c>
       <c r="U3" t="n">
-        <v>1283</v>
+        <v>1283.41999</v>
       </c>
     </row>
     <row r="4">
@@ -750,7 +750,7 @@
         <v>100</v>
       </c>
       <c r="U4" t="n">
-        <v>1255</v>
+        <v>1255.15376</v>
       </c>
     </row>
     <row r="5">
@@ -1900,7 +1900,7 @@
         <v>62.5</v>
       </c>
       <c r="U2" t="n">
-        <v>1299</v>
+        <v>1299.09471</v>
       </c>
       <c r="V2" t="n">
         <v>5.25656078379703</v>
@@ -1992,7 +1992,7 @@
         <v>128</v>
       </c>
       <c r="U3" t="n">
-        <v>1283</v>
+        <v>1283.41999</v>
       </c>
       <c r="V3" t="n">
         <v>5.41772022250839</v>
@@ -2084,7 +2084,7 @@
         <v>100</v>
       </c>
       <c r="U4" t="n">
-        <v>1255</v>
+        <v>1255.15376</v>
       </c>
       <c r="V4" t="n">
         <v>5.35342092765938</v>
@@ -3523,7 +3523,7 @@
         <v>62.5</v>
       </c>
       <c r="U2" t="n">
-        <v>1299</v>
+        <v>1299.09471</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
@@ -3616,7 +3616,7 @@
         <v>128</v>
       </c>
       <c r="U3" t="n">
-        <v>1283</v>
+        <v>1283.41999</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
@@ -3709,7 +3709,7 @@
         <v>100</v>
       </c>
       <c r="U4" t="n">
-        <v>1255</v>
+        <v>1255.15376</v>
       </c>
       <c r="V4" t="n">
         <v>0</v>
@@ -5100,13 +5100,13 @@
         <v>62.5</v>
       </c>
       <c r="U2" t="n">
-        <v>1299</v>
+        <v>1299.09471</v>
       </c>
       <c r="V2" t="n">
-        <v>0.474057358911017</v>
+        <v>0.474060274275901</v>
       </c>
       <c r="W2" t="n">
-        <v>0.525942641088983</v>
+        <v>0.525939725724099</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
@@ -5183,7 +5183,7 @@
         <v>128</v>
       </c>
       <c r="U3" t="n">
-        <v>1283</v>
+        <v>1283.41999</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
@@ -5270,7 +5270,7 @@
         <v>100</v>
       </c>
       <c r="U4" t="n">
-        <v>1255</v>
+        <v>1255.15376</v>
       </c>
       <c r="V4" t="n">
         <v>0</v>
@@ -6601,25 +6601,25 @@
         <v>62.5</v>
       </c>
       <c r="U2" t="n">
-        <v>1299</v>
+        <v>1299.09471</v>
       </c>
       <c r="V2" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="W2" t="n">
         <v>925</v>
       </c>
       <c r="X2" t="n">
-        <v>0.416371110659367</v>
+        <v>0.469913142701622</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.583628889340633</v>
+        <v>0.530086857298378</v>
       </c>
       <c r="Z2" t="n">
-        <v>0</v>
+        <v>0.000835660852316802</v>
       </c>
       <c r="AA2" t="n">
-        <v>0</v>
+        <v>0.0008356608523168019</v>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
@@ -6696,7 +6696,7 @@
         <v>128</v>
       </c>
       <c r="U3" t="n">
-        <v>1283</v>
+        <v>1283.41999</v>
       </c>
       <c r="V3" t="n">
         <v>130</v>
@@ -6711,10 +6711,10 @@
         <v>0.7844709533493121</v>
       </c>
       <c r="Z3" t="n">
-        <v>0</v>
+        <v>3.75646222415579e-05</v>
       </c>
       <c r="AA3" t="n">
-        <v>0</v>
+        <v>3.756462224155789e-05</v>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
@@ -6791,25 +6791,25 @@
         <v>100</v>
       </c>
       <c r="U4" t="n">
-        <v>1255</v>
+        <v>1255.15376</v>
       </c>
       <c r="V4" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="W4" t="n">
         <v>925</v>
       </c>
       <c r="X4" t="n">
-        <v>0.271684996651186</v>
+        <v>0.29235352352064</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.728315003348814</v>
+        <v>0.70764647647936</v>
       </c>
       <c r="Z4" t="n">
-        <v>0</v>
+        <v>0.000634775486311526</v>
       </c>
       <c r="AA4" t="n">
-        <v>0</v>
+        <v>0.0006347754863115258</v>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
@@ -6889,22 +6889,22 @@
         <v>1200</v>
       </c>
       <c r="V5" t="n">
-        <v>2510</v>
+        <v>2500</v>
       </c>
       <c r="W5" t="n">
         <v>925</v>
       </c>
       <c r="X5" t="n">
-        <v>0.795267495209578</v>
+        <v>0.796513677120962</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.204732504790422</v>
+        <v>0.203486322879038</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>0.00123226570304335</v>
       </c>
       <c r="AA5" t="n">
-        <v>0</v>
+        <v>0.00123226570304335</v>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
@@ -6990,16 +6990,16 @@
         <v>925</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8367329263408561</v>
+        <v>0.836894576666795</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.163267073659144</v>
+        <v>0.163105423333205</v>
       </c>
       <c r="Z6" t="n">
-        <v>0</v>
+        <v>0.000226271338451074</v>
       </c>
       <c r="AA6" t="n">
-        <v>0</v>
+        <v>0.0002262713384510739</v>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
@@ -7091,10 +7091,10 @@
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>0</v>
+        <v>0.0129029986829266</v>
       </c>
       <c r="AA7" t="n">
-        <v>0</v>
+        <v>0.01290299868292659</v>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
@@ -7186,10 +7186,10 @@
         <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>0</v>
+        <v>0.00105217920776629</v>
       </c>
       <c r="AA8" t="n">
-        <v>0</v>
+        <v>0.00105217920776629</v>
       </c>
       <c r="AB8" t="inlineStr">
         <is>
@@ -7269,7 +7269,7 @@
         <v>1050</v>
       </c>
       <c r="V9" t="n">
-        <v>2550</v>
+        <v>2540</v>
       </c>
       <c r="W9" t="n">
         <v>925</v>
@@ -7281,10 +7281,10 @@
         <v>0</v>
       </c>
       <c r="Z9" t="n">
-        <v>0</v>
+        <v>0.0160925216776623</v>
       </c>
       <c r="AA9" t="n">
-        <v>0</v>
+        <v>0.01609252167766231</v>
       </c>
       <c r="AB9" t="inlineStr">
         <is>
@@ -7364,22 +7364,22 @@
         <v>900</v>
       </c>
       <c r="V10" t="n">
-        <v>1110</v>
+        <v>1100</v>
       </c>
       <c r="W10" t="n">
         <v>925</v>
       </c>
       <c r="X10" t="n">
-        <v>0.970537500959608</v>
+        <v>0.972472424256134</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.0294624990403915</v>
+        <v>0.0275275757438659</v>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
+        <v>0.007924265844899119</v>
       </c>
       <c r="AA10" t="n">
-        <v>0</v>
+        <v>0.007924265844899111</v>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
@@ -7459,22 +7459,22 @@
         <v>900</v>
       </c>
       <c r="V11" t="n">
-        <v>1800</v>
+        <v>1790</v>
       </c>
       <c r="W11" t="n">
         <v>925</v>
       </c>
       <c r="X11" t="n">
-        <v>0.972103309419704</v>
+        <v>0.972874630367114</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.0278966905802956</v>
+        <v>0.0271253696328862</v>
       </c>
       <c r="Z11" t="n">
-        <v>0</v>
+        <v>0.00667100825932183</v>
       </c>
       <c r="AA11" t="n">
-        <v>0</v>
+        <v>0.006671008259321829</v>
       </c>
       <c r="AB11" t="inlineStr">
         <is>
@@ -7554,22 +7554,22 @@
         <v>900</v>
       </c>
       <c r="V12" t="n">
-        <v>1740</v>
+        <v>1730</v>
       </c>
       <c r="W12" t="n">
         <v>925</v>
       </c>
       <c r="X12" t="n">
-        <v>0.974688169297985</v>
+        <v>0.97561394228405</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.025311830702015</v>
+        <v>0.0243860577159497</v>
       </c>
       <c r="Z12" t="n">
-        <v>0</v>
+        <v>0.008636970211907451</v>
       </c>
       <c r="AA12" t="n">
-        <v>0</v>
+        <v>0.008636970211907449</v>
       </c>
       <c r="AB12" t="inlineStr">
         <is>
@@ -7649,22 +7649,22 @@
         <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>2100</v>
+        <v>2090</v>
       </c>
       <c r="W13" t="n">
         <v>925</v>
       </c>
       <c r="X13" t="n">
-        <v>0.950654147209229</v>
+        <v>0.951891002202502</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.0493458527907711</v>
+        <v>0.048108997797498</v>
       </c>
       <c r="Z13" t="n">
-        <v>0</v>
+        <v>0.00294119534061353</v>
       </c>
       <c r="AA13" t="n">
-        <v>0</v>
+        <v>0.002941195340613532</v>
       </c>
       <c r="AB13" t="inlineStr">
         <is>
@@ -7744,22 +7744,22 @@
         <v>900</v>
       </c>
       <c r="V14" t="n">
-        <v>1740</v>
+        <v>1730</v>
       </c>
       <c r="W14" t="n">
         <v>925</v>
       </c>
       <c r="X14" t="n">
-        <v>0.949126162299477</v>
+        <v>0.950741498987455</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.050873837700523</v>
+        <v>0.0492585010125445</v>
       </c>
       <c r="Z14" t="n">
-        <v>0</v>
+        <v>0.00286390060466055</v>
       </c>
       <c r="AA14" t="n">
-        <v>0</v>
+        <v>0.002863900604660548</v>
       </c>
       <c r="AB14" t="inlineStr">
         <is>
@@ -7845,16 +7845,16 @@
         <v>925</v>
       </c>
       <c r="X15" t="n">
-        <v>0.231707821017839</v>
+        <v>0.231707821016213</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.768292178982161</v>
+        <v>0.768292178983787</v>
       </c>
       <c r="Z15" t="n">
-        <v>0</v>
+        <v>9.309173835698601e-05</v>
       </c>
       <c r="AA15" t="n">
-        <v>0</v>
+        <v>9.309173835698606e-05</v>
       </c>
       <c r="AB15" t="inlineStr">
         <is>
@@ -7940,16 +7940,16 @@
         <v>925</v>
       </c>
       <c r="X16" t="n">
-        <v>0.456496184913214</v>
+        <v>0.456749735218006</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.543503815086786</v>
+        <v>0.543250264781994</v>
       </c>
       <c r="Z16" t="n">
-        <v>0</v>
+        <v>0.000938033056325138</v>
       </c>
       <c r="AA16" t="n">
-        <v>0</v>
+        <v>0.0009380330563251388</v>
       </c>
       <c r="AB16" t="inlineStr">
         <is>
@@ -8035,16 +8035,16 @@
         <v>925</v>
       </c>
       <c r="X17" t="n">
-        <v>0.684461157687705</v>
+        <v>0.684728944146793</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.315538842312295</v>
+        <v>0.315271055853207</v>
       </c>
       <c r="Z17" t="n">
-        <v>0</v>
+        <v>0.000430867551518525</v>
       </c>
       <c r="AA17" t="n">
-        <v>0</v>
+        <v>0.0004308675515185249</v>
       </c>
       <c r="AB17" t="inlineStr">
         <is>
@@ -8277,22 +8277,22 @@
         <v>62.5</v>
       </c>
       <c r="U2" t="n">
-        <v>1299</v>
+        <v>1299.09471</v>
       </c>
       <c r="V2" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="W2" t="n">
-        <v>0.456384672752863</v>
+        <v>0.493184396428161</v>
       </c>
       <c r="X2" t="n">
-        <v>0.543615327247137</v>
+        <v>0.506815603571839</v>
       </c>
       <c r="Y2" t="n">
-        <v>0</v>
+        <v>0.000609818056595781</v>
       </c>
       <c r="Z2" t="n">
-        <v>0</v>
+        <v>0.000609818056595781</v>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
@@ -8369,22 +8369,22 @@
         <v>128</v>
       </c>
       <c r="U3" t="n">
-        <v>1283</v>
+        <v>1283.41999</v>
       </c>
       <c r="V3" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="W3" t="n">
-        <v>0.251373285069106</v>
+        <v>0.266594556578593</v>
       </c>
       <c r="X3" t="n">
-        <v>0.7486267149308941</v>
+        <v>0.733405443421407</v>
       </c>
       <c r="Y3" t="n">
-        <v>0</v>
+        <v>0.000699690455656429</v>
       </c>
       <c r="Z3" t="n">
-        <v>0</v>
+        <v>0.0006996904556564294</v>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
@@ -8461,22 +8461,22 @@
         <v>100</v>
       </c>
       <c r="U4" t="n">
-        <v>1255</v>
+        <v>1255.15376</v>
       </c>
       <c r="V4" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="W4" t="n">
-        <v>0.308244721446847</v>
+        <v>0.337738175495508</v>
       </c>
       <c r="X4" t="n">
-        <v>0.691755278553153</v>
+        <v>0.662261824504492</v>
       </c>
       <c r="Y4" t="n">
-        <v>0</v>
+        <v>0.000807422690952036</v>
       </c>
       <c r="Z4" t="n">
-        <v>0</v>
+        <v>0.0008074226909520355</v>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
@@ -8556,19 +8556,19 @@
         <v>1200</v>
       </c>
       <c r="V5" t="n">
-        <v>2550</v>
+        <v>2540</v>
       </c>
       <c r="W5" t="n">
-        <v>0.8162510061536929</v>
+        <v>0.817547776604673</v>
       </c>
       <c r="X5" t="n">
-        <v>0.183748993846307</v>
+        <v>0.182452223395327</v>
       </c>
       <c r="Y5" t="n">
-        <v>0</v>
+        <v>0.0015319426079297</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>0.0015319426079297</v>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
@@ -8651,16 +8651,16 @@
         <v>2850</v>
       </c>
       <c r="W6" t="n">
-        <v>0.854729032250732</v>
+        <v>0.8552141507186199</v>
       </c>
       <c r="X6" t="n">
-        <v>0.145270967749268</v>
+        <v>0.14478584928138</v>
       </c>
       <c r="Y6" t="n">
-        <v>0</v>
+        <v>0.000849378234060265</v>
       </c>
       <c r="Z6" t="n">
-        <v>0</v>
+        <v>0.0008493782340602644</v>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
@@ -8749,10 +8749,10 @@
         <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>0</v>
+        <v>0.00344178052689819</v>
       </c>
       <c r="Z7" t="n">
-        <v>0</v>
+        <v>0.003441780526898187</v>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
@@ -8832,7 +8832,7 @@
         <v>1100</v>
       </c>
       <c r="V8" t="n">
-        <v>1660</v>
+        <v>1650</v>
       </c>
       <c r="W8" t="n">
         <v>1</v>
@@ -8841,10 +8841,10 @@
         <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>0</v>
+        <v>0.0152803231983435</v>
       </c>
       <c r="Z8" t="n">
-        <v>0</v>
+        <v>0.01528032319834351</v>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
@@ -8933,10 +8933,10 @@
         <v>0</v>
       </c>
       <c r="Y9" t="n">
-        <v>0</v>
+        <v>0.008153007612025051</v>
       </c>
       <c r="Z9" t="n">
-        <v>0</v>
+        <v>0.008153007612025049</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
@@ -9016,19 +9016,19 @@
         <v>900</v>
       </c>
       <c r="V10" t="n">
-        <v>1100</v>
+        <v>1090</v>
       </c>
       <c r="W10" t="n">
-        <v>0.9710120167797061</v>
+        <v>0.972915709108933</v>
       </c>
       <c r="X10" t="n">
-        <v>0.0289879832202938</v>
+        <v>0.0270842908910666</v>
       </c>
       <c r="Y10" t="n">
-        <v>0</v>
+        <v>0.00885469016241785</v>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
+        <v>0.008854690162417838</v>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
@@ -9108,19 +9108,19 @@
         <v>900</v>
       </c>
       <c r="V11" t="n">
-        <v>1790</v>
+        <v>1780</v>
       </c>
       <c r="W11" t="n">
-        <v>0.972527926335185</v>
+        <v>0.973132721034933</v>
       </c>
       <c r="X11" t="n">
-        <v>0.0274720736648147</v>
+        <v>0.0268672789650666</v>
       </c>
       <c r="Y11" t="n">
-        <v>0</v>
+        <v>0.00591552141542247</v>
       </c>
       <c r="Z11" t="n">
-        <v>0</v>
+        <v>0.005915521415422469</v>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
@@ -9200,19 +9200,19 @@
         <v>900</v>
       </c>
       <c r="V12" t="n">
-        <v>1730</v>
+        <v>1720</v>
       </c>
       <c r="W12" t="n">
-        <v>0.974950805204835</v>
+        <v>0.975859890544081</v>
       </c>
       <c r="X12" t="n">
-        <v>0.0250491947951647</v>
+        <v>0.0241401094559188</v>
       </c>
       <c r="Y12" t="n">
-        <v>0</v>
+        <v>0.00808765212115037</v>
       </c>
       <c r="Z12" t="n">
-        <v>0</v>
+        <v>0.008087652121150367</v>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
@@ -9378,19 +9378,19 @@
         <v>900</v>
       </c>
       <c r="V14" t="n">
-        <v>1740</v>
+        <v>1730</v>
       </c>
       <c r="W14" t="n">
-        <v>0.948904090216909</v>
+        <v>0.951016786572314</v>
       </c>
       <c r="X14" t="n">
-        <v>0.0510959097830914</v>
+        <v>0.048983213427686</v>
       </c>
       <c r="Y14" t="n">
-        <v>0</v>
+        <v>0.00335004855562078</v>
       </c>
       <c r="Z14" t="n">
-        <v>0</v>
+        <v>0.003350048555620779</v>
       </c>
       <c r="AA14" t="inlineStr">
         <is>
@@ -9470,19 +9470,19 @@
         <v>1050</v>
       </c>
       <c r="V15" t="n">
-        <v>1290</v>
+        <v>1280</v>
       </c>
       <c r="W15" t="n">
-        <v>0.227348245202519</v>
+        <v>0.228644415713756</v>
       </c>
       <c r="X15" t="n">
-        <v>0.772651754797481</v>
+        <v>0.771355584286244</v>
       </c>
       <c r="Y15" t="n">
-        <v>0</v>
+        <v>0.00147492657477965</v>
       </c>
       <c r="Z15" t="n">
-        <v>0</v>
+        <v>0.00147492657477965</v>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
@@ -9562,19 +9562,19 @@
         <v>1000</v>
       </c>
       <c r="V16" t="n">
-        <v>4920</v>
+        <v>4910</v>
       </c>
       <c r="W16" t="n">
-        <v>0.45836885367988</v>
+        <v>0.458904496315431</v>
       </c>
       <c r="X16" t="n">
-        <v>0.541631146320119</v>
+        <v>0.541095503684569</v>
       </c>
       <c r="Y16" t="n">
-        <v>0</v>
+        <v>0.00176716229182296</v>
       </c>
       <c r="Z16" t="n">
-        <v>0</v>
+        <v>0.001767162291822961</v>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
@@ -9654,19 +9654,19 @@
         <v>1100</v>
       </c>
       <c r="V17" t="n">
-        <v>1600</v>
+        <v>1590</v>
       </c>
       <c r="W17" t="n">
-        <v>0.678292384823151</v>
+        <v>0.679642799711047</v>
       </c>
       <c r="X17" t="n">
-        <v>0.321707615176849</v>
+        <v>0.320357200288953</v>
       </c>
       <c r="Y17" t="n">
-        <v>0</v>
+        <v>0.00191408285739597</v>
       </c>
       <c r="Z17" t="n">
-        <v>0</v>
+        <v>0.00191408285739597</v>
       </c>
       <c r="AA17" t="inlineStr">
         <is>

</xml_diff>